<commit_message>
Add validation for write permissions when sharing a file
</commit_message>
<xml_diff>
--- a/users/root/uploads/test.xlsx
+++ b/users/root/uploads/test.xlsx
@@ -980,7 +980,7 @@
     </row>
     <row r="2" spans="1:8" customHeight="1" ht="12.75">
       <c r="A2" s="1">
-        <v>61639123</v>
+        <v>61639</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="3" spans="1:8" customHeight="1" ht="12.75">
       <c r="A3" s="1">
-        <v>61876</v>
+        <v>618763</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>

</xml_diff>